<commit_message>
check box problem solved
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -903,7 +903,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1032,11 +1032,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="172974464"/>
-        <c:axId val="172976000"/>
+        <c:axId val="95974912"/>
+        <c:axId val="82761920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172974464"/>
+        <c:axId val="95974912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172976000"/>
+        <c:crossAx val="82761920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1054,7 +1054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172976000"/>
+        <c:axId val="82761920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1065,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172974464"/>
+        <c:crossAx val="95974912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1089,7 +1089,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1221,11 +1221,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="172532096"/>
-        <c:axId val="172533632"/>
+        <c:axId val="85685760"/>
+        <c:axId val="95535104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172532096"/>
+        <c:axId val="85685760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1235,7 +1235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172533632"/>
+        <c:crossAx val="95535104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1243,7 +1243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172533632"/>
+        <c:axId val="95535104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172532096"/>
+        <c:crossAx val="85685760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1285,7 +1285,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="tr-TR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1414,11 +1414,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="172594688"/>
-        <c:axId val="172596224"/>
+        <c:axId val="95688704"/>
+        <c:axId val="95536832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172594688"/>
+        <c:axId val="95688704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172596224"/>
+        <c:crossAx val="95536832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1436,7 +1436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172596224"/>
+        <c:axId val="95536832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172594688"/>
+        <c:crossAx val="95688704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2754,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,11 +2976,11 @@
       <c r="F16" s="2">
         <v>6</v>
       </c>
-      <c r="G16" s="43" t="s">
-        <v>72</v>
+      <c r="G16" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="H16" s="42">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J16" s="23" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
updated Product & Sprint Backlog
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration-1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="108">
   <si>
     <t>STORY</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Product Backlog Items</t>
   </si>
   <si>
-    <t>Estimated Completion Time (hrs)</t>
-  </si>
-  <si>
     <t>Actual Time Spend (hrs)</t>
   </si>
   <si>
@@ -309,6 +306,42 @@
   </si>
   <si>
     <t>New Spring Backlog</t>
+  </si>
+  <si>
+    <t>Room No generated automatically</t>
+  </si>
+  <si>
+    <t>GamzeKüçükçolak</t>
+  </si>
+  <si>
+    <t>Display students according to the enrolled rooms</t>
+  </si>
+  <si>
+    <t>View student information on profile tab</t>
+  </si>
+  <si>
+    <t>#7.5</t>
+  </si>
+  <si>
+    <t>#3.3</t>
+  </si>
+  <si>
+    <t>#14.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design GUI (chart data type) </t>
+  </si>
+  <si>
+    <t>#14.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design new GUI (show dorm capacity) </t>
+  </si>
+  <si>
+    <t>#14.4</t>
+  </si>
+  <si>
+    <t>Check the occupancy of rooms in DB at a given time interval</t>
   </si>
 </sst>
 </file>
@@ -1032,11 +1065,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95974912"/>
-        <c:axId val="82761920"/>
+        <c:axId val="120157696"/>
+        <c:axId val="91412672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95974912"/>
+        <c:axId val="120157696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1079,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82761920"/>
+        <c:crossAx val="91412672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1054,7 +1087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82761920"/>
+        <c:axId val="91412672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95974912"/>
+        <c:crossAx val="120157696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1221,11 +1254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85685760"/>
-        <c:axId val="95535104"/>
+        <c:axId val="95192576"/>
+        <c:axId val="119717888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85685760"/>
+        <c:axId val="95192576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1235,7 +1268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95535104"/>
+        <c:crossAx val="119717888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1243,7 +1276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95535104"/>
+        <c:axId val="119717888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85685760"/>
+        <c:crossAx val="95192576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1345,7 +1378,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration-1'!$P$26:$U$26</c:f>
+              <c:f>'Iteration-2'!$P$26:$U$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1356,7 +1389,7 @@
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>26</c:v>
@@ -1389,15 +1422,18 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Iteration-1'!$P$25:$Q$25</c:f>
+              <c:f>'Iteration-2'!$N$38:$N$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,11 +1450,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95688704"/>
-        <c:axId val="95536832"/>
+        <c:axId val="119871488"/>
+        <c:axId val="119719616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95688704"/>
+        <c:axId val="119871488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1464,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95536832"/>
+        <c:crossAx val="119719616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1436,7 +1472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95536832"/>
+        <c:axId val="119719616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,13 +1483,20 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95688704"/>
+        <c:crossAx val="119871488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1706,38 +1749,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -1815,6 +1826,38 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>721178</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>71436</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2231,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J13" s="23" t="s">
         <v>14</v>
@@ -2263,7 +2306,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H14" s="42">
         <v>0.7</v>
@@ -2674,10 +2717,10 @@
         <v>67</v>
       </c>
       <c r="Q30" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S30" s="41"/>
     </row>
@@ -2727,7 +2770,7 @@
     </row>
     <row r="35" spans="16:18" x14ac:dyDescent="0.25">
       <c r="P35" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q35">
         <f>SUM(Q31:Q34)</f>
@@ -2754,8 +2797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="C8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,13 +2920,13 @@
         <v>2</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J13" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>23</v>
@@ -2915,10 +2958,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>31</v>
@@ -2948,10 +2991,10 @@
       </c>
       <c r="H15" s="42"/>
       <c r="J15" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>31</v>
@@ -2976,17 +3019,17 @@
       <c r="F16" s="2">
         <v>6</v>
       </c>
-      <c r="G16" s="34" t="s">
-        <v>66</v>
+      <c r="G16" s="52" t="s">
+        <v>71</v>
       </c>
       <c r="H16" s="42">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>24</v>
@@ -3016,13 +3059,13 @@
       </c>
       <c r="H17" s="42"/>
       <c r="J17" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="M17" s="14">
         <v>2</v>
@@ -3051,10 +3094,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>22</v>
@@ -3084,10 +3127,10 @@
       </c>
       <c r="H19" s="42"/>
       <c r="J19" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>23</v>
@@ -3119,10 +3162,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>25</v>
@@ -3152,10 +3195,10 @@
       </c>
       <c r="H21" s="42"/>
       <c r="J21" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L21" s="26" t="s">
         <v>22</v>
@@ -3181,7 +3224,7 @@
         <v>12</v>
       </c>
       <c r="G22" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="42">
         <v>0.4</v>
@@ -3246,7 +3289,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M24" s="59">
         <v>4</v>
@@ -3326,10 +3369,10 @@
     </row>
     <row r="27" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="50" t="s">
         <v>82</v>
-      </c>
-      <c r="D27" s="50" t="s">
-        <v>83</v>
       </c>
       <c r="E27" s="51">
         <v>3</v>
@@ -3338,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="G27" s="57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H27" s="55">
         <v>0.5</v>
@@ -3379,13 +3422,13 @@
         <v>67</v>
       </c>
       <c r="Q30" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="R30" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="S30" s="41" t="s">
         <v>93</v>
-      </c>
-      <c r="R30" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="S30" s="41" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="31" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3465,7 +3508,7 @@
     </row>
     <row r="36" spans="14:19" x14ac:dyDescent="0.25">
       <c r="P36" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q36">
         <f>SUM(Q31:Q35)</f>
@@ -3518,10 +3561,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U35"/>
+  <dimension ref="B2:U38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,7 +3578,7 @@
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
-    <col min="11" max="11" width="41.140625" customWidth="1"/>
+    <col min="11" max="11" width="50.7109375" customWidth="1"/>
     <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
@@ -3642,15 +3685,19 @@
         <v>2</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="23"/>
-      <c r="K13" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="L13" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="M13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N13" s="35" t="s">
         <v>66</v>
@@ -3675,10 +3722,14 @@
       <c r="H14" s="42">
         <v>1</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1" t="s">
-        <v>24</v>
+      <c r="J14" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="M14" s="2">
         <v>2</v>
@@ -3704,13 +3755,17 @@
         <v>4</v>
       </c>
       <c r="H15" s="42"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="11"/>
+      <c r="J15" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>99</v>
+      </c>
       <c r="L15" s="1" t="s">
         <v>31</v>
       </c>
       <c r="M15" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="35" t="s">
         <v>66</v>
@@ -3729,14 +3784,18 @@
       <c r="F16" s="2">
         <v>6</v>
       </c>
-      <c r="G16" s="43" t="s">
-        <v>72</v>
+      <c r="G16" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="H16" s="42">
-        <v>0.6</v>
-      </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="L16" s="1" t="s">
         <v>22</v>
       </c>
@@ -3764,13 +3823,17 @@
         <v>4</v>
       </c>
       <c r="H17" s="42"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="1"/>
+      <c r="J17" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="L17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M17" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N17" s="35" t="s">
         <v>66</v>
@@ -3795,10 +3858,14 @@
       <c r="H18" s="42">
         <v>1</v>
       </c>
-      <c r="J18" s="24"/>
-      <c r="K18" s="1"/>
+      <c r="J18" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="L18" s="13" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="M18" s="14">
         <v>2</v>
@@ -3807,7 +3874,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C19" s="23" t="s">
         <v>9</v>
       </c>
@@ -3824,17 +3891,17 @@
         <v>4</v>
       </c>
       <c r="H19" s="42"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="27"/>
-      <c r="N19" s="47" t="s">
+      <c r="J19" s="23"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="35" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="23" t="s">
         <v>10</v>
       </c>
@@ -3853,16 +3920,21 @@
       <c r="H20" s="42">
         <v>1</v>
       </c>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="6">
-        <f>SUM(M13:M19)</f>
-        <v>12</v>
-      </c>
-      <c r="N20" s="17"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="27"/>
+      <c r="N20" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="P20">
+        <v>65</v>
+      </c>
+      <c r="Q20">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C21" s="23" t="s">
@@ -3881,6 +3953,16 @@
         <v>4</v>
       </c>
       <c r="H21" s="42"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="6">
+        <f>SUM(M13:M20)</f>
+        <v>9</v>
+      </c>
+      <c r="N21" s="17"/>
     </row>
     <row r="22" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C22" s="23" t="s">
@@ -3895,15 +3977,19 @@
       <c r="F22" s="2">
         <v>12</v>
       </c>
-      <c r="G22" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="42"/>
+      <c r="G22" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="42">
+        <v>0.4</v>
+      </c>
       <c r="P22">
+        <f>P23</f>
         <v>65</v>
       </c>
       <c r="Q22">
-        <v>44</v>
+        <f>P22-R34</f>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="3:21" x14ac:dyDescent="0.25">
@@ -3927,7 +4013,14 @@
       <c r="K23" s="17"/>
       <c r="L23" s="18"/>
       <c r="M23" s="19"/>
-      <c r="N23" s="17"/>
+      <c r="P23">
+        <f>P24</f>
+        <v>65</v>
+      </c>
+      <c r="Q23">
+        <f>Q24+(R34-Q34)</f>
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C24" s="23" t="s">
@@ -3949,12 +4042,24 @@
         <v>1</v>
       </c>
       <c r="P24">
-        <f>P25</f>
         <v>65</v>
       </c>
       <c r="Q24">
-        <f>P24-R35</f>
-        <v>44</v>
+        <f>P24-17</f>
+        <v>48</v>
+      </c>
+      <c r="R24">
+        <f>Q24-M21+4</f>
+        <v>43</v>
+      </c>
+      <c r="S24">
+        <v>26</v>
+      </c>
+      <c r="T24">
+        <v>13</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:21" x14ac:dyDescent="0.25">
@@ -3970,157 +4075,207 @@
       <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G25" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="42"/>
-      <c r="P25">
-        <f>P26</f>
-        <v>65</v>
-      </c>
-      <c r="Q25">
-        <f>Q26+(R35-Q35)</f>
-        <v>52</v>
+      <c r="G25" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="42">
+        <v>1</v>
+      </c>
+      <c r="P25" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="R25" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="U25" s="32" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="2">
         <v>3</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="2">
         <v>10</v>
       </c>
-      <c r="G26" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" s="42">
+      <c r="G26" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="42"/>
+    </row>
+    <row r="27" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="30">
+        <v>3</v>
+      </c>
+      <c r="F27" s="30">
+        <v>4</v>
+      </c>
+      <c r="G27" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" s="42">
         <v>0.2</v>
       </c>
-      <c r="P26">
-        <f>F27</f>
+    </row>
+    <row r="28" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="17"/>
+      <c r="D28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="4">
+        <f>SUM(F14:F27)</f>
+        <v>69</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="P28" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q28" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="R28" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="S28" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="38">
+        <v>8</v>
+      </c>
+      <c r="R29" s="39">
+        <v>13</v>
+      </c>
+      <c r="S29">
+        <f>R29-SUM('Iteration-1'!M12:M13)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P30" s="40">
+        <v>7</v>
+      </c>
+      <c r="Q30" s="39">
+        <v>4</v>
+      </c>
+      <c r="R30" s="39">
+        <v>8</v>
+      </c>
+      <c r="S30">
+        <f>R30-SUM('Iteration-1'!M14:M16)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P31" s="38">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="39">
+        <v>6</v>
+      </c>
+      <c r="R31" s="39">
+        <v>4</v>
+      </c>
+      <c r="S31">
+        <f>R31</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P32" s="38">
+        <v>9</v>
+      </c>
+      <c r="Q32" s="39">
+        <v>12</v>
+      </c>
+      <c r="R32" s="39">
+        <v>4</v>
+      </c>
+      <c r="S32">
+        <f>R32</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P33" s="38">
+        <v>14</v>
+      </c>
+      <c r="Q33" s="39">
+        <v>4</v>
+      </c>
+      <c r="R33" s="39">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <f>R33</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P34" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q34">
+        <f>SUM(Q29:Q33)</f>
+        <v>34</v>
+      </c>
+      <c r="R34">
+        <f>SUM(R29:R33)</f>
+        <v>31</v>
+      </c>
+      <c r="S34">
+        <f>SUM(S29:S33)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N36">
         <v>65</v>
       </c>
-      <c r="Q26">
-        <f>P26-17</f>
-        <v>48</v>
-      </c>
-      <c r="R26">
-        <v>39</v>
-      </c>
-      <c r="S26">
-        <v>26</v>
-      </c>
-      <c r="T26">
-        <v>13</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C27" s="17"/>
-      <c r="D27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="4">
-        <f>SUM(F14:F26)</f>
+      <c r="O36">
         <v>65</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="P27" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q27" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="R27" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="S27" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="T27" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="U27" s="32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P30" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q30" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="R30" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="S30" s="41"/>
-    </row>
-    <row r="31" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P31" s="37">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="38">
-        <v>8</v>
-      </c>
-      <c r="R31" s="39">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P32" s="40">
-        <v>7</v>
-      </c>
-      <c r="Q32" s="39">
-        <v>4</v>
-      </c>
-      <c r="R32" s="39">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="16:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P33" s="38">
-        <v>5</v>
-      </c>
-      <c r="Q33" s="39">
-        <v>2</v>
-      </c>
-      <c r="R33" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="16:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P34" s="38">
-        <v>11</v>
-      </c>
-      <c r="Q34" s="39">
-        <v>3</v>
-      </c>
-      <c r="R34" s="39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P35" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q35">
-        <f>SUM(Q31:Q34)</f>
-        <v>17</v>
-      </c>
-      <c r="R35">
-        <f>SUM(R31:R34)</f>
-        <v>21</v>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="53"/>
+    </row>
+    <row r="37" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>52</v>
+      </c>
+      <c r="O37">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <f>N37-S34+M22</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4130,7 +4285,8 @@
     <mergeCell ref="C12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
all changes and search all
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration-1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Iteration-3" sheetId="3" r:id="rId3"/>
     <sheet name="Iteration-4" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration-5" sheetId="5" r:id="rId5"/>
+    <sheet name="Iteration-6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="145">
   <si>
     <t>STORY</t>
   </si>
@@ -381,6 +382,78 @@
   </si>
   <si>
     <t>WEEK6</t>
+  </si>
+  <si>
+    <t>#9.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter students with respect to name </t>
+  </si>
+  <si>
+    <t>Nazli Karalar</t>
+  </si>
+  <si>
+    <t>#13.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorm and room can be changed </t>
+  </si>
+  <si>
+    <t>Kağan Kayaalp</t>
+  </si>
+  <si>
+    <t>#14.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorm capacity chart </t>
+  </si>
+  <si>
+    <t>#6.1</t>
+  </si>
+  <si>
+    <t>#4.1</t>
+  </si>
+  <si>
+    <t>#4.2</t>
+  </si>
+  <si>
+    <t>Add Damaged Item GUI</t>
+  </si>
+  <si>
+    <t>Add Lost Item GUI</t>
+  </si>
+  <si>
+    <t>#4.3</t>
+  </si>
+  <si>
+    <t>#4.4</t>
+  </si>
+  <si>
+    <t>Items List GUI</t>
+  </si>
+  <si>
+    <t>Damaged/Lost/Closed Items Procedures</t>
+  </si>
+  <si>
+    <t>#4.5</t>
+  </si>
+  <si>
+    <t>Closed Item GUI</t>
+  </si>
+  <si>
+    <t>Ismetcan Hergünsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment GUI </t>
+  </si>
+  <si>
+    <t>#4.6</t>
+  </si>
+  <si>
+    <t>Lost and Damaged Items can be closed</t>
+  </si>
+  <si>
+    <t>Nazli Karalar &amp; Erdi Koç</t>
   </si>
 </sst>
 </file>
@@ -488,7 +561,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -842,12 +915,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -958,6 +1044,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -970,10 +1063,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,11 +1218,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="120740352"/>
-        <c:axId val="120358592"/>
+        <c:axId val="95847936"/>
+        <c:axId val="85252288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="120740352"/>
+        <c:axId val="95847936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1140,7 +1232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120358592"/>
+        <c:crossAx val="85252288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1148,7 +1240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120358592"/>
+        <c:axId val="85252288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,7 +1251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120740352"/>
+        <c:crossAx val="95847936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1316,11 +1408,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="57428480"/>
-        <c:axId val="120360320"/>
+        <c:axId val="87598592"/>
+        <c:axId val="95469568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57428480"/>
+        <c:axId val="87598592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,7 +1422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120360320"/>
+        <c:crossAx val="95469568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1338,7 +1430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120360320"/>
+        <c:axId val="95469568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57428480"/>
+        <c:crossAx val="87598592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1362,7 +1454,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1518,11 +1609,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="120782336"/>
-        <c:axId val="120362048"/>
+        <c:axId val="95565824"/>
+        <c:axId val="95471296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="120782336"/>
+        <c:axId val="95565824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1532,7 +1623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120362048"/>
+        <c:crossAx val="95471296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1540,7 +1631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120362048"/>
+        <c:axId val="95471296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1642,244 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120782336"/>
+        <c:crossAx val="95565824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="tr-TR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Task Remaining</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Iteration-4'!$P$25:$V$25</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>START</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WEEK1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WEEK2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WEEK3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WEEK4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WEEK5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WEEK6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration-3'!$P$24:$V$24</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.833333333333323</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Tasks Remaining</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Iteration-4'!$P$25:$V$25</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>START</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WEEK1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WEEK2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WEEK3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WEEK4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WEEK5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WEEK6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration-4'!$P$23:$T$23</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="42660864"/>
+        <c:axId val="96833472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="42660864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96833472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96833472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42660864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1931,6 +2259,124 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1609725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3952875" y="885824"/>
+          <a:ext cx="5715000" cy="1066801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="F1FCBC"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="1"/>
+            <a:t>Description:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DMS is a desktop application which enables dormitory managers to track students living in their dorms.They will be able to enter students' registrations including student's information (names, surnames, e-mails etc), residents' fees, debts and also they can define the room types and their prices. Besides, this program shows the room of the students and their start/end dates of staying in the dorm.</a:t>
+          </a:r>
+          <a:endParaRPr lang="tr-TR" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>721178</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>71436</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2245,14 +2691,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2291,22 +2737,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="63" t="s">
+      <c r="J11" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
       <c r="H12" s="33"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -2891,14 +3337,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2937,23 +3383,23 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="65" t="s">
+      <c r="J11" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="67"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="70"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="70"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
       </c>
@@ -3631,8 +4077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="H10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23:S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3656,14 +4102,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3702,22 +4148,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="63" t="s">
+      <c r="J11" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
       <c r="H12" s="48"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -3900,7 +4346,7 @@
       <c r="L17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="68">
+      <c r="M17" s="64">
         <v>1</v>
       </c>
       <c r="N17" s="35" t="s">
@@ -4127,7 +4573,7 @@
         <f>P24</f>
         <v>65</v>
       </c>
-      <c r="Q23" s="69">
+      <c r="Q23" s="65">
         <f>Q24+(R35-Q35)</f>
         <v>56.166666666666664</v>
       </c>
@@ -4161,27 +4607,27 @@
       <c r="P24">
         <v>65</v>
       </c>
-      <c r="Q24" s="69">
+      <c r="Q24" s="65">
         <f>P24-Q17</f>
         <v>54.166666666666664</v>
       </c>
-      <c r="R24" s="69">
+      <c r="R24" s="65">
         <f>Q24-Q17</f>
         <v>43.333333333333329</v>
       </c>
-      <c r="S24" s="69">
+      <c r="S24" s="65">
         <f>R24-Q17</f>
         <v>32.499999999999993</v>
       </c>
-      <c r="T24" s="69">
+      <c r="T24" s="65">
         <f>S24-Q17</f>
         <v>21.666666666666657</v>
       </c>
-      <c r="U24" s="69">
+      <c r="U24" s="65">
         <f>T24-Q17</f>
         <v>10.833333333333323</v>
       </c>
-      <c r="V24" s="69">
+      <c r="V24" s="65">
         <f>U24-Q17</f>
         <v>0</v>
       </c>
@@ -4446,15 +4892,818 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V46" sqref="V46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J11" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+    </row>
+    <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="63"/>
+      <c r="J12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="N13" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="42">
+        <v>1</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="N14" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="42"/>
+      <c r="J15" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="L15" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="M15" s="12">
+        <v>2</v>
+      </c>
+      <c r="N15" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>6</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="42">
+        <v>1</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M16" s="14">
+        <v>1</v>
+      </c>
+      <c r="N16" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C17" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="42">
+        <v>1</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L17" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="M17" s="64">
+        <v>1</v>
+      </c>
+      <c r="N17" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q17">
+        <f>65/6</f>
+        <v>10.833333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="42">
+        <v>1</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" s="14">
+        <v>1</v>
+      </c>
+      <c r="N18" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>4</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="42">
+        <v>0.3</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L19" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="M19" s="2">
+        <v>2</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>4</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="42">
+        <v>1</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="P20">
+        <v>65</v>
+      </c>
+      <c r="Q20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="42"/>
+      <c r="J21" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M21" s="64">
+        <v>2</v>
+      </c>
+      <c r="N21" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2">
+        <v>12</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="42">
+        <v>1</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L22" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="M22" s="27">
+        <v>1</v>
+      </c>
+      <c r="N22" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22">
+        <f>P23</f>
+        <v>65</v>
+      </c>
+      <c r="Q22">
+        <f>P22-R35</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C23" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="42">
+        <v>1</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" s="6">
+        <f>SUM(M13:M22)</f>
+        <v>13</v>
+      </c>
+      <c r="N23" s="17"/>
+      <c r="P23">
+        <f>P24</f>
+        <v>65</v>
+      </c>
+      <c r="Q23" s="65">
+        <f>Q24+(R35-Q35)</f>
+        <v>57.166666666666664</v>
+      </c>
+      <c r="R23">
+        <v>41</v>
+      </c>
+      <c r="S23">
+        <v>25</v>
+      </c>
+      <c r="T23">
+        <f>S23-(Q35+S35)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="42">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>65</v>
+      </c>
+      <c r="Q24" s="65">
+        <f>P24-Q17</f>
+        <v>54.166666666666664</v>
+      </c>
+      <c r="R24" s="65">
+        <f>Q24-Q17</f>
+        <v>43.333333333333329</v>
+      </c>
+      <c r="S24" s="65">
+        <f>R24-Q17</f>
+        <v>32.499999999999993</v>
+      </c>
+      <c r="T24" s="65">
+        <f>S24-Q17</f>
+        <v>21.666666666666657</v>
+      </c>
+      <c r="U24" s="65">
+        <f>T24-Q17</f>
+        <v>10.833333333333323</v>
+      </c>
+      <c r="V24" s="65">
+        <f>U24-Q17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C25" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="42">
+        <v>1</v>
+      </c>
+      <c r="P25" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="R25" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="U25" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="V25" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="15">
+        <v>3</v>
+      </c>
+      <c r="F26" s="15">
+        <v>5</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4</v>
+      </c>
+      <c r="F27" s="2">
+        <v>4</v>
+      </c>
+      <c r="G27" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" s="42">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="30">
+        <v>4</v>
+      </c>
+      <c r="F28" s="30">
+        <v>5</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="62"/>
+      <c r="P28" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q28" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="R28" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="S28" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="17"/>
+      <c r="D29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="4">
+        <f>SUM(F14:F28)</f>
+        <v>69</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="P29" s="37">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="38">
+        <v>6</v>
+      </c>
+      <c r="R29" s="39">
+        <v>8</v>
+      </c>
+      <c r="S29">
+        <f>Q29-R29</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P30" s="40">
+        <v>6</v>
+      </c>
+      <c r="Q30" s="39">
+        <v>4</v>
+      </c>
+      <c r="R30" s="39">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <f t="shared" ref="S30:S34" si="0">Q30-R30</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P31" s="38">
+        <v>9</v>
+      </c>
+      <c r="Q31" s="39">
+        <v>0</v>
+      </c>
+      <c r="R31" s="39">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P32" s="38">
+        <v>13</v>
+      </c>
+      <c r="Q32" s="39">
+        <v>0</v>
+      </c>
+      <c r="R32" s="39">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P33" s="38">
+        <v>14</v>
+      </c>
+      <c r="Q33" s="39">
+        <v>0</v>
+      </c>
+      <c r="R33" s="39">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="34" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P34" s="38"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P35" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q35">
+        <f>SUM(Q29:Q34)</f>
+        <v>10</v>
+      </c>
+      <c r="R35">
+        <f>SUM(R29:R34)</f>
+        <v>13</v>
+      </c>
+      <c r="S35">
+        <f>SUM(S29:S34)</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="36" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>65</v>
+      </c>
+      <c r="O36">
+        <v>65</v>
+      </c>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="53"/>
+    </row>
+    <row r="37" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>52</v>
+      </c>
+      <c r="O37">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="C12:G12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4468,4 +5717,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
unused codes deleted, search all works
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="150">
   <si>
     <t>STORY</t>
   </si>
@@ -454,6 +454,21 @@
   </si>
   <si>
     <t>Nazli Karalar &amp; Erdi Koç</t>
+  </si>
+  <si>
+    <t>Male/Female Chart</t>
+  </si>
+  <si>
+    <t>Erdi Koç &amp; Gamze</t>
+  </si>
+  <si>
+    <t>#16</t>
+  </si>
+  <si>
+    <t>Show male/female capacity</t>
+  </si>
+  <si>
+    <t>#15.1</t>
   </si>
 </sst>
 </file>
@@ -561,7 +576,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -928,12 +943,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1048,6 +1156,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1063,9 +1174,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,11 +1339,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95847936"/>
-        <c:axId val="85252288"/>
+        <c:axId val="133134848"/>
+        <c:axId val="88201984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95847936"/>
+        <c:axId val="133134848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1232,7 +1353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85252288"/>
+        <c:crossAx val="88201984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1240,7 +1361,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85252288"/>
+        <c:axId val="88201984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,14 +1372,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95847936"/>
+        <c:crossAx val="133134848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1408,11 +1528,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="87598592"/>
-        <c:axId val="95469568"/>
+        <c:axId val="100833792"/>
+        <c:axId val="100958784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87598592"/>
+        <c:axId val="100833792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95469568"/>
+        <c:crossAx val="100958784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1430,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95469568"/>
+        <c:axId val="100958784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1441,7 +1561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87598592"/>
+        <c:crossAx val="100833792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1454,6 +1574,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1609,11 +1730,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95565824"/>
-        <c:axId val="95471296"/>
+        <c:axId val="101027328"/>
+        <c:axId val="100960512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95565824"/>
+        <c:axId val="101027328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,7 +1744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95471296"/>
+        <c:crossAx val="100960512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1631,7 +1752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95471296"/>
+        <c:axId val="100960512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95565824"/>
+        <c:crossAx val="101027328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1820,7 +1941,7 @@
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.166666666666664</c:v>
+                  <c:v>58.166666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>41</c:v>
@@ -1829,7 +1950,7 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1846,11 +1967,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42660864"/>
-        <c:axId val="96833472"/>
+        <c:axId val="101025792"/>
+        <c:axId val="100962240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42660864"/>
+        <c:axId val="101025792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1860,7 +1981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96833472"/>
+        <c:crossAx val="100962240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1868,7 +1989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96833472"/>
+        <c:axId val="100962240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,7 +2000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42660864"/>
+        <c:crossAx val="101025792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2691,14 +2812,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2737,22 +2858,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="33"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -3337,14 +3458,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3383,23 +3504,23 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="70"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="73"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="70"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="73"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
       </c>
@@ -4077,8 +4198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V37"/>
   <sheetViews>
-    <sheetView topLeftCell="H10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23:S23"/>
+    <sheetView topLeftCell="G10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4102,14 +4223,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4148,22 +4269,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="48"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -4894,8 +5015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V46" sqref="V46"/>
+    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4917,14 +5038,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" ht="22.5" x14ac:dyDescent="0.35">
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4963,22 +5084,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="63"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -5010,10 +5131,10 @@
       <c r="F13" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="80" t="s">
         <v>70</v>
       </c>
       <c r="J13" s="23" t="s">
@@ -5045,10 +5166,10 @@
       <c r="F14" s="2">
         <v>8</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="42">
+      <c r="G14" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="54">
         <v>1</v>
       </c>
       <c r="J14" s="23" t="s">
@@ -5080,10 +5201,10 @@
       <c r="F15" s="2">
         <v>3</v>
       </c>
-      <c r="G15" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="42"/>
+      <c r="G15" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="54"/>
       <c r="J15" s="24" t="s">
         <v>127</v>
       </c>
@@ -5113,10 +5234,10 @@
       <c r="F16" s="2">
         <v>6</v>
       </c>
-      <c r="G16" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="42">
+      <c r="G16" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="54">
         <v>1</v>
       </c>
       <c r="J16" s="24" t="s">
@@ -5148,10 +5269,10 @@
       <c r="F17" s="2">
         <v>6</v>
       </c>
-      <c r="G17" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="42">
+      <c r="G17" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="54">
         <v>1</v>
       </c>
       <c r="J17" s="24" t="s">
@@ -5160,7 +5281,7 @@
       <c r="K17" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="L17" s="71" t="s">
+      <c r="L17" s="66" t="s">
         <v>112</v>
       </c>
       <c r="M17" s="64">
@@ -5187,10 +5308,10 @@
       <c r="F18" s="2">
         <v>2</v>
       </c>
-      <c r="G18" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="42">
+      <c r="G18" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="54">
         <v>1</v>
       </c>
       <c r="J18" s="24" t="s">
@@ -5222,10 +5343,10 @@
       <c r="F19" s="2">
         <v>4</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="42">
+      <c r="H19" s="54">
         <v>0.3</v>
       </c>
       <c r="J19" s="23" t="s">
@@ -5234,7 +5355,7 @@
       <c r="K19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L19" s="72" t="s">
+      <c r="L19" s="67" t="s">
         <v>112</v>
       </c>
       <c r="M19" s="2">
@@ -5257,10 +5378,10 @@
       <c r="F20" s="2">
         <v>4</v>
       </c>
-      <c r="G20" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="42">
+      <c r="G20" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="54">
         <v>1</v>
       </c>
       <c r="J20" s="23" t="s">
@@ -5298,10 +5419,12 @@
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="G21" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="42"/>
+      <c r="G21" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="54">
+        <v>1</v>
+      </c>
       <c r="J21" s="24" t="s">
         <v>142</v>
       </c>
@@ -5318,7 +5441,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C22" s="23" t="s">
         <v>12</v>
       </c>
@@ -5331,25 +5454,25 @@
       <c r="F22" s="2">
         <v>12</v>
       </c>
-      <c r="G22" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="42">
-        <v>1</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="K22" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="L22" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="M22" s="27">
-        <v>1</v>
-      </c>
-      <c r="N22" s="47" t="s">
+      <c r="G22" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="54">
+        <v>1</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M22" s="64">
+        <v>1</v>
+      </c>
+      <c r="N22" s="35" t="s">
         <v>66</v>
       </c>
       <c r="P22">
@@ -5358,10 +5481,10 @@
       </c>
       <c r="Q22">
         <f>P22-R35</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="23" t="s">
         <v>13</v>
       </c>
@@ -5374,29 +5497,32 @@
       <c r="F23" s="2">
         <v>4</v>
       </c>
-      <c r="G23" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="42">
-        <v>1</v>
-      </c>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="6">
-        <f>SUM(M13:M22)</f>
-        <v>13</v>
-      </c>
-      <c r="N23" s="17"/>
+      <c r="G23" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="54"/>
+      <c r="J23" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="K23" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L23" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="M23" s="27">
+        <v>1</v>
+      </c>
+      <c r="N23" s="47" t="s">
+        <v>66</v>
+      </c>
       <c r="P23">
         <f>P24</f>
         <v>65</v>
       </c>
       <c r="Q23" s="65">
         <f>Q24+(R35-Q35)</f>
-        <v>57.166666666666664</v>
+        <v>58.166666666666664</v>
       </c>
       <c r="R23">
         <v>41</v>
@@ -5405,8 +5531,8 @@
         <v>25</v>
       </c>
       <c r="T23">
-        <f>S23-(Q35+S35)</f>
-        <v>18</v>
+        <f>S23-M24+4</f>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.25">
@@ -5422,12 +5548,22 @@
       <c r="F24" s="2">
         <v>3</v>
       </c>
-      <c r="G24" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="42">
-        <v>1</v>
-      </c>
+      <c r="G24" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="82">
+        <v>1</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="6">
+        <f>SUM(M13:M23)</f>
+        <v>14</v>
+      </c>
+      <c r="N24" s="17"/>
       <c r="P24">
         <v>65</v>
       </c>
@@ -5469,10 +5605,10 @@
       <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G25" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="42">
+      <c r="G25" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="54">
         <v>1</v>
       </c>
       <c r="P25" s="32" t="s">
@@ -5510,10 +5646,10 @@
       <c r="F26" s="15">
         <v>5</v>
       </c>
-      <c r="G26" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" s="42">
+      <c r="G26" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="54">
         <v>1</v>
       </c>
     </row>
@@ -5530,30 +5666,32 @@
       <c r="F27" s="2">
         <v>4</v>
       </c>
-      <c r="G27" s="43" t="s">
+      <c r="G27" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>3</v>
+      </c>
+      <c r="G28" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="42">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="28" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="30">
-        <v>4</v>
-      </c>
-      <c r="F28" s="30">
-        <v>5</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="62"/>
+      <c r="H28" s="54">
+        <v>0.8</v>
+      </c>
       <c r="P28" s="44" t="s">
         <v>67</v>
       </c>
@@ -5568,16 +5706,22 @@
       </c>
     </row>
     <row r="29" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="17"/>
-      <c r="D29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="4">
-        <f>SUM(F14:F28)</f>
-        <v>69</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
+      <c r="C29" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="30">
+        <v>4</v>
+      </c>
+      <c r="F29" s="30">
+        <v>5</v>
+      </c>
+      <c r="G29" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="81"/>
       <c r="P29" s="37">
         <v>4</v>
       </c>
@@ -5593,6 +5737,16 @@
       </c>
     </row>
     <row r="30" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="17"/>
+      <c r="D30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="4">
+        <f>SUM(F14:F29)</f>
+        <v>72</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
       <c r="P30" s="40">
         <v>6</v>
       </c>
@@ -5603,7 +5757,7 @@
         <v>1</v>
       </c>
       <c r="S30">
-        <f t="shared" ref="S30:S34" si="0">Q30-R30</f>
+        <f>Q30-R30</f>
         <v>3</v>
       </c>
     </row>
@@ -5618,7 +5772,7 @@
         <v>1</v>
       </c>
       <c r="S31">
-        <f t="shared" si="0"/>
+        <f>Q31-R31</f>
         <v>-1</v>
       </c>
     </row>
@@ -5633,7 +5787,7 @@
         <v>1</v>
       </c>
       <c r="S32">
-        <f t="shared" si="0"/>
+        <f>Q32-R32</f>
         <v>-1</v>
       </c>
     </row>
@@ -5645,20 +5799,26 @@
         <v>0</v>
       </c>
       <c r="R33" s="39">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <f>Q33-R33</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P34" s="38">
+        <v>15</v>
+      </c>
+      <c r="Q34" s="39">
+        <v>0</v>
+      </c>
+      <c r="R34" s="39">
         <v>2</v>
       </c>
-      <c r="S33">
-        <f t="shared" si="0"/>
+      <c r="S34">
+        <f>Q34-R34</f>
         <v>-2</v>
-      </c>
-    </row>
-    <row r="34" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P34" s="38"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="39"/>
-      <c r="S34">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="35" spans="14:19" x14ac:dyDescent="0.25">
@@ -5671,11 +5831,11 @@
       </c>
       <c r="R35">
         <f>SUM(R29:R34)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S35">
         <f>SUM(S29:S34)</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="36" spans="14:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
search all gui done
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -1159,6 +1159,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1172,19 +1185,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1339,11 +1339,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133134848"/>
-        <c:axId val="88201984"/>
+        <c:axId val="110258688"/>
+        <c:axId val="94887232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133134848"/>
+        <c:axId val="110258688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88201984"/>
+        <c:crossAx val="94887232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1361,7 +1361,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88201984"/>
+        <c:axId val="94887232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133134848"/>
+        <c:crossAx val="110258688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1528,11 +1528,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100833792"/>
-        <c:axId val="100958784"/>
+        <c:axId val="110360064"/>
+        <c:axId val="109855296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100833792"/>
+        <c:axId val="110360064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1542,7 +1542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100958784"/>
+        <c:crossAx val="109855296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1550,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100958784"/>
+        <c:axId val="109855296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100833792"/>
+        <c:crossAx val="110360064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1574,7 +1574,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1730,11 +1729,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101027328"/>
-        <c:axId val="100960512"/>
+        <c:axId val="110358528"/>
+        <c:axId val="109857024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101027328"/>
+        <c:axId val="110358528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +1743,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100960512"/>
+        <c:crossAx val="109857024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1752,7 +1751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100960512"/>
+        <c:axId val="109857024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1762,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101027328"/>
+        <c:crossAx val="110358528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1941,7 +1940,7 @@
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58.166666666666664</c:v>
+                  <c:v>57.166666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>41</c:v>
@@ -1950,7 +1949,7 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1967,11 +1966,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101025792"/>
-        <c:axId val="100962240"/>
+        <c:axId val="111036416"/>
+        <c:axId val="109858752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101025792"/>
+        <c:axId val="111036416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1981,7 +1980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100962240"/>
+        <c:crossAx val="109858752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1989,7 +1988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100962240"/>
+        <c:axId val="109858752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,7 +1999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101025792"/>
+        <c:crossAx val="111036416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2812,14 +2811,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2858,22 +2857,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
       <c r="H12" s="33"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -3458,14 +3457,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3504,23 +3503,23 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="71" t="s">
+      <c r="J11" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="73"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="82"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="73"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="82"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
       </c>
@@ -4223,14 +4222,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4269,22 +4268,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
       <c r="H12" s="48"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -5015,8 +5014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5038,14 +5037,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" ht="22.5" x14ac:dyDescent="0.35">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5084,22 +5083,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
       <c r="H12" s="63"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -5131,10 +5130,10 @@
       <c r="F13" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="74" t="s">
+      <c r="G13" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="80" t="s">
+      <c r="H13" s="75" t="s">
         <v>70</v>
       </c>
       <c r="J13" s="23" t="s">
@@ -5166,7 +5165,7 @@
       <c r="F14" s="2">
         <v>8</v>
       </c>
-      <c r="G14" s="75" t="s">
+      <c r="G14" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H14" s="54">
@@ -5201,7 +5200,7 @@
       <c r="F15" s="2">
         <v>3</v>
       </c>
-      <c r="G15" s="76" t="s">
+      <c r="G15" s="71" t="s">
         <v>4</v>
       </c>
       <c r="H15" s="54"/>
@@ -5234,7 +5233,7 @@
       <c r="F16" s="2">
         <v>6</v>
       </c>
-      <c r="G16" s="75" t="s">
+      <c r="G16" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H16" s="54">
@@ -5269,7 +5268,7 @@
       <c r="F17" s="2">
         <v>6</v>
       </c>
-      <c r="G17" s="75" t="s">
+      <c r="G17" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H17" s="54">
@@ -5308,7 +5307,7 @@
       <c r="F18" s="2">
         <v>2</v>
       </c>
-      <c r="G18" s="75" t="s">
+      <c r="G18" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H18" s="54">
@@ -5343,7 +5342,7 @@
       <c r="F19" s="2">
         <v>4</v>
       </c>
-      <c r="G19" s="77" t="s">
+      <c r="G19" s="72" t="s">
         <v>71</v>
       </c>
       <c r="H19" s="54">
@@ -5378,7 +5377,7 @@
       <c r="F20" s="2">
         <v>4</v>
       </c>
-      <c r="G20" s="75" t="s">
+      <c r="G20" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="54">
@@ -5419,7 +5418,7 @@
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="G21" s="75" t="s">
+      <c r="G21" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H21" s="54">
@@ -5454,7 +5453,7 @@
       <c r="F22" s="2">
         <v>12</v>
       </c>
-      <c r="G22" s="75" t="s">
+      <c r="G22" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H22" s="54">
@@ -5470,7 +5469,7 @@
         <v>146</v>
       </c>
       <c r="M22" s="64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N22" s="35" t="s">
         <v>66</v>
@@ -5497,7 +5496,7 @@
       <c r="F23" s="2">
         <v>4</v>
       </c>
-      <c r="G23" s="76" t="s">
+      <c r="G23" s="71" t="s">
         <v>4</v>
       </c>
       <c r="H23" s="54"/>
@@ -5522,7 +5521,7 @@
       </c>
       <c r="Q23" s="65">
         <f>Q24+(R35-Q35)</f>
-        <v>58.166666666666664</v>
+        <v>57.166666666666664</v>
       </c>
       <c r="R23">
         <v>41</v>
@@ -5531,8 +5530,8 @@
         <v>25</v>
       </c>
       <c r="T23">
-        <f>S23-M24+4</f>
-        <v>15</v>
+        <f>S23-M24+3</f>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.25">
@@ -5548,10 +5547,10 @@
       <c r="F24" s="2">
         <v>3</v>
       </c>
-      <c r="G24" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="82">
+      <c r="G24" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="77">
         <v>1</v>
       </c>
       <c r="J24" s="17"/>
@@ -5561,7 +5560,7 @@
       </c>
       <c r="M24" s="6">
         <f>SUM(M13:M23)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N24" s="17"/>
       <c r="P24">
@@ -5605,7 +5604,7 @@
       <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G25" s="75" t="s">
+      <c r="G25" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H25" s="54">
@@ -5646,7 +5645,7 @@
       <c r="F26" s="15">
         <v>5</v>
       </c>
-      <c r="G26" s="75" t="s">
+      <c r="G26" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H26" s="54">
@@ -5666,7 +5665,7 @@
       <c r="F27" s="2">
         <v>4</v>
       </c>
-      <c r="G27" s="75" t="s">
+      <c r="G27" s="70" t="s">
         <v>66</v>
       </c>
       <c r="H27" s="54">
@@ -5684,9 +5683,9 @@
         <v>4</v>
       </c>
       <c r="F28" s="2">
-        <v>3</v>
-      </c>
-      <c r="G28" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="72" t="s">
         <v>71</v>
       </c>
       <c r="H28" s="54">
@@ -5718,10 +5717,10 @@
       <c r="F29" s="30">
         <v>5</v>
       </c>
-      <c r="G29" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="81"/>
+      <c r="G29" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="76"/>
       <c r="P29" s="37">
         <v>4</v>
       </c>
@@ -5732,7 +5731,7 @@
         <v>8</v>
       </c>
       <c r="S29">
-        <f>Q29-R29</f>
+        <f t="shared" ref="S29:S34" si="0">Q29-R29</f>
         <v>-2</v>
       </c>
     </row>
@@ -5743,7 +5742,7 @@
       </c>
       <c r="F30" s="4">
         <f>SUM(F14:F29)</f>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -5757,7 +5756,7 @@
         <v>1</v>
       </c>
       <c r="S30">
-        <f>Q30-R30</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -5772,7 +5771,7 @@
         <v>1</v>
       </c>
       <c r="S31">
-        <f>Q31-R31</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
@@ -5787,7 +5786,7 @@
         <v>1</v>
       </c>
       <c r="S32">
-        <f>Q32-R32</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
@@ -5802,7 +5801,7 @@
         <v>1</v>
       </c>
       <c r="S33">
-        <f>Q33-R33</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
@@ -5811,14 +5810,14 @@
         <v>15</v>
       </c>
       <c r="Q34" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" s="39">
         <v>2</v>
       </c>
       <c r="S34">
-        <f>Q34-R34</f>
-        <v>-2</v>
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="35" spans="14:19" x14ac:dyDescent="0.25">
@@ -5827,7 +5826,7 @@
       </c>
       <c r="Q35">
         <f>SUM(Q29:Q34)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R35">
         <f>SUM(R29:R34)</f>
@@ -5835,7 +5834,7 @@
       </c>
       <c r="S35">
         <f>SUM(S29:S34)</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="36" spans="14:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
all changes, updates, payment...
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration-1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="163">
   <si>
     <t>STORY</t>
   </si>
@@ -469,12 +469,54 @@
   </si>
   <si>
     <t>#15.1</t>
+  </si>
+  <si>
+    <t>#15.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male/female capacity </t>
+  </si>
+  <si>
+    <t>WEEK5 SUM</t>
+  </si>
+  <si>
+    <t>#13.4</t>
+  </si>
+  <si>
+    <t>Added Undo feature to the update student</t>
+  </si>
+  <si>
+    <t>#1.7</t>
+  </si>
+  <si>
+    <t>#4.7</t>
+  </si>
+  <si>
+    <t>#13.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dates are updated </t>
+  </si>
+  <si>
+    <t>#6.2</t>
+  </si>
+  <si>
+    <t>Payment cash is done</t>
+  </si>
+  <si>
+    <t>Added filter with respect to dorms, rooms, date</t>
+  </si>
+  <si>
+    <t>#8.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₺_-;\-* #,##0.00\ _₺_-;_-* &quot;-&quot;??\ _₺_-;_-@_-"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1037,11 +1079,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1175,6 +1218,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1187,8 +1233,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1339,11 +1389,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110258688"/>
-        <c:axId val="94887232"/>
+        <c:axId val="108890112"/>
+        <c:axId val="96787776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110258688"/>
+        <c:axId val="108890112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94887232"/>
+        <c:crossAx val="96787776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1361,7 +1411,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94887232"/>
+        <c:axId val="96787776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110258688"/>
+        <c:crossAx val="108890112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1528,11 +1578,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110360064"/>
-        <c:axId val="109855296"/>
+        <c:axId val="98347008"/>
+        <c:axId val="108741184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110360064"/>
+        <c:axId val="98347008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1542,7 +1592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109855296"/>
+        <c:crossAx val="108741184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1550,7 +1600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109855296"/>
+        <c:axId val="108741184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110360064"/>
+        <c:crossAx val="98347008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1574,6 +1624,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1729,11 +1780,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110358528"/>
-        <c:axId val="109857024"/>
+        <c:axId val="108891648"/>
+        <c:axId val="108742912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110358528"/>
+        <c:axId val="108891648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1743,7 +1794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109857024"/>
+        <c:crossAx val="108742912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1751,7 +1802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109857024"/>
+        <c:axId val="108742912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110358528"/>
+        <c:crossAx val="108891648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1949,7 +2000,7 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>13</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1966,11 +2017,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111036416"/>
-        <c:axId val="109858752"/>
+        <c:axId val="109135872"/>
+        <c:axId val="108744640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111036416"/>
+        <c:axId val="109135872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,7 +2031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109858752"/>
+        <c:crossAx val="108744640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1988,7 +2039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109858752"/>
+        <c:axId val="108744640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +2050,247 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111036416"/>
+        <c:crossAx val="109135872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="tr-TR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Task Remaining</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Iteration-4'!$P$25:$V$25</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>START</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WEEK1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WEEK2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WEEK3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WEEK4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WEEK5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WEEK6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration-3'!$P$24:$V$24</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.833333333333323</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Tasks Remaining</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Iteration-4'!$P$25:$V$25</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>START</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WEEK1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WEEK2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>WEEK3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>WEEK4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>WEEK5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WEEK6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Iteration-5'!$P$23:$U$23</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="87703552"/>
+        <c:axId val="85399744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="87703552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85399744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85399744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87703552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2497,6 +2788,124 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1609725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3533775" y="914399"/>
+          <a:ext cx="5505450" cy="1066801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="F1FCBC"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="1"/>
+            <a:t>Description:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DMS is a desktop application which enables dormitory managers to track students living in their dorms.They will be able to enter students' registrations including student's information (names, surnames, e-mails etc), residents' fees, debts and also they can define the room types and their prices. Besides, this program shows the room of the students and their start/end dates of staying in the dorm.</a:t>
+          </a:r>
+          <a:endParaRPr lang="tr-TR" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>721178</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>71436</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2811,14 +3220,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2857,22 +3266,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="78" t="s">
+      <c r="J11" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="33"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -3457,14 +3866,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3503,23 +3912,23 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="80" t="s">
+      <c r="J11" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="83"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="80" t="s">
+      <c r="C12" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="83"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
       </c>
@@ -4222,14 +4631,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4268,22 +4677,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="78" t="s">
+      <c r="J11" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="48"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -5014,8 +5423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView topLeftCell="G3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5037,14 +5446,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:15" ht="22.5" x14ac:dyDescent="0.35">
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5083,22 +5492,22 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J11" s="78" t="s">
+      <c r="J11" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
     </row>
     <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="63"/>
       <c r="J12" s="20" t="s">
         <v>17</v>
@@ -5530,8 +5939,8 @@
         <v>25</v>
       </c>
       <c r="T23">
-        <f>S23-M24+3</f>
-        <v>13</v>
+        <f>S23-M24+3+F29</f>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.25">
@@ -5868,13 +6277,770 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J11" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
+    </row>
+    <row r="12" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="78"/>
+      <c r="J12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="N13" s="35"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8</v>
+      </c>
+      <c r="G14" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="54">
+        <v>1</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="84">
+        <v>2</v>
+      </c>
+      <c r="N14" s="35"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="J15" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="L15" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" s="35"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>6</v>
+      </c>
+      <c r="G16" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="54">
+        <v>1</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L16" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="35"/>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C17" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6</v>
+      </c>
+      <c r="G17" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="54">
+        <v>1</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="L17" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="35"/>
+      <c r="Q17">
+        <f>65/6</f>
+        <v>10.833333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="54">
+        <v>1</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" s="14">
+        <v>2</v>
+      </c>
+      <c r="N18" s="35"/>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>4</v>
+      </c>
+      <c r="G19" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="54">
+        <v>0.8</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L19" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="2">
+        <v>2</v>
+      </c>
+      <c r="N19" s="35"/>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>4</v>
+      </c>
+      <c r="G20" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="54">
+        <v>1</v>
+      </c>
+      <c r="J20" s="23"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="35"/>
+      <c r="P20">
+        <v>65</v>
+      </c>
+      <c r="Q20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="54">
+        <v>1</v>
+      </c>
+      <c r="J21" s="24"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="35"/>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C22" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2">
+        <v>12</v>
+      </c>
+      <c r="G22" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="54">
+        <v>1</v>
+      </c>
+      <c r="J22" s="24"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="35"/>
+      <c r="P22">
+        <f>P23</f>
+        <v>65</v>
+      </c>
+      <c r="Q22">
+        <f>P22-R35</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4</v>
+      </c>
+      <c r="G23" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="54"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="47"/>
+      <c r="P23">
+        <f>P24</f>
+        <v>65</v>
+      </c>
+      <c r="Q23" s="65">
+        <f>Q24+(R35-Q35)</f>
+        <v>54.166666666666664</v>
+      </c>
+      <c r="R23">
+        <v>41</v>
+      </c>
+      <c r="S23">
+        <v>25</v>
+      </c>
+      <c r="T23">
+        <v>18</v>
+      </c>
+      <c r="U23">
+        <f>T23-M24+7</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="77">
+        <v>1</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" s="6">
+        <f>SUM(M13:M23)</f>
+        <v>10</v>
+      </c>
+      <c r="N24" s="17"/>
+      <c r="P24">
+        <v>65</v>
+      </c>
+      <c r="Q24" s="65">
+        <f>P24-Q17</f>
+        <v>54.166666666666664</v>
+      </c>
+      <c r="R24" s="65">
+        <f>Q24-Q17</f>
+        <v>43.333333333333329</v>
+      </c>
+      <c r="S24" s="65">
+        <f>R24-Q17</f>
+        <v>32.499999999999993</v>
+      </c>
+      <c r="T24" s="65">
+        <f>S24-Q17</f>
+        <v>21.666666666666657</v>
+      </c>
+      <c r="U24" s="65">
+        <f>T24-Q17</f>
+        <v>10.833333333333323</v>
+      </c>
+      <c r="V24" s="65">
+        <f>U24-Q17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C25" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="54">
+        <v>1</v>
+      </c>
+      <c r="P25" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="R25" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="U25" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="V25" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="15">
+        <v>3</v>
+      </c>
+      <c r="F26" s="15">
+        <v>5</v>
+      </c>
+      <c r="G26" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4</v>
+      </c>
+      <c r="F27" s="2">
+        <v>4</v>
+      </c>
+      <c r="G27" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="54">
+        <v>1</v>
+      </c>
+      <c r="P28" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q28" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="R28" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="S28" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="30">
+        <v>4</v>
+      </c>
+      <c r="F29" s="30">
+        <v>5</v>
+      </c>
+      <c r="G29" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="76"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="39"/>
+      <c r="S29">
+        <f t="shared" ref="S29:S34" si="0">Q29-R29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="17"/>
+      <c r="D30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="4">
+        <f>SUM(F14:F29)</f>
+        <v>70</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="39"/>
+      <c r="R30" s="39"/>
+      <c r="S30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P31" s="38"/>
+      <c r="Q31" s="39"/>
+      <c r="R31" s="39"/>
+      <c r="S31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P32" s="38"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39"/>
+      <c r="S32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P33" s="38"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="39"/>
+      <c r="S33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P34" s="38"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P35" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q35">
+        <f>SUM(Q29:Q34)</f>
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <f>SUM(R29:R34)</f>
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <f>SUM(S29:S34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>65</v>
+      </c>
+      <c r="O36">
+        <v>65</v>
+      </c>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="53"/>
+    </row>
+    <row r="37" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>52</v>
+      </c>
+      <c r="O37">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="C12:G12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>